<commit_message>
make a file that can handle the extra price for the island
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsTax.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsTax.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/SuppXLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_AD4D1D646341095ACB700054E557F514683EDF16" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{465E415E-98DC-4663-9E79-61F2B0E8DB8D}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_AD4D1D646341095ACB700054E557F514683EDF16" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA88F2C0-2BDC-4933-95B9-A3D3C54DAE1C}"/>
   <bookViews>
-    <workbookView xWindow="-27030" yWindow="6720" windowWidth="16875" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27030" yWindow="675" windowWidth="16875" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -58,6 +58,30 @@
   </si>
   <si>
     <t>NCAP_ITAX</t>
+  </si>
+  <si>
+    <t>DKISLBH</t>
+  </si>
+  <si>
+    <t>DKISL1</t>
+  </si>
+  <si>
+    <t>DKISL2</t>
+  </si>
+  <si>
+    <t>DKISL3</t>
+  </si>
+  <si>
+    <t>ERWINELCWIN3N</t>
+  </si>
+  <si>
+    <t>ERWINELCWIN5N</t>
+  </si>
+  <si>
+    <t>CURR</t>
+  </si>
+  <si>
+    <t>Mkr20</t>
   </si>
 </sst>
 </file>
@@ -65,9 +89,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,12 +118,6 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -121,7 +139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -140,6 +158,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -152,7 +185,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal 2" xfId="1" xr:uid="{99D0E672-6040-42DE-8EA8-FDE4967F2131}"/>
@@ -438,7 +471,7 @@
   <dimension ref="B4:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -477,17 +510,27 @@
       <c r="E5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="J5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="4"/>
+      <c r="L5" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -496,13 +539,41 @@
       <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="5"/>
+      <c r="G6" s="5">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="H6" s="5">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="I6" s="5">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="J6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.45">
       <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="5"/>
+      <c r="G7" s="5">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="I7" s="5">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix mistake regarding currency
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsTax.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsTax.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/SuppXLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_AD4D1D646341095ACB700054E557F514683EDF16" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA88F2C0-2BDC-4933-95B9-A3D3C54DAE1C}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="11_AD4D1D646341095ACB700054E557F514683EDF16" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{918A3676-67C8-4899-A362-75B46C65A16F}"/>
   <bookViews>
-    <workbookView xWindow="-27030" yWindow="675" windowWidth="16875" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44880" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
     <t>CURR</t>
   </si>
   <si>
-    <t>Mkr20</t>
+    <t>MKr20</t>
   </si>
 </sst>
 </file>
@@ -89,7 +89,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -185,7 +185,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal 2" xfId="1" xr:uid="{99D0E672-6040-42DE-8EA8-FDE4967F2131}"/>
@@ -470,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="152" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Update of UPD table
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_EnergyIslandsTax.xlsx
+++ b/SuppXLS/Scen_ELC_EnergyIslandsTax.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/SuppXLS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_AD4D1D646341095ACB700054E557F514683EDF16" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{918A3676-67C8-4899-A362-75B46C65A16F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7005B22-66F6-4579-A654-0DE762E5BF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44880" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
-    <t>~TFM_UPD</t>
-  </si>
-  <si>
     <t>TimeSlice</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>MKr20</t>
+  </si>
+  <si>
+    <t>~TFM_INS</t>
   </si>
 </sst>
 </file>
@@ -188,9 +188,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{99D0E672-6040-42DE-8EA8-FDE4967F2131}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{9FC41D72-367E-4602-B746-F5D4903E59B9}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -470,18 +470,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="152" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" zoomScale="152" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -497,47 +497,47 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="2:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="L5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G6" s="5">
         <v>1.0900000000000001</v>
@@ -549,15 +549,15 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="J6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G7" s="5">
         <v>1.0900000000000001</v>
@@ -569,10 +569,10 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="J7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>